<commit_message>
hoan tra diem tich luy khi update, xoa, them
</commit_message>
<xml_diff>
--- a/HoaDon.xlsx
+++ b/HoaDon.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\PharmacyManage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3464A7-4979-4845-8A3C-52FA9ED6ABEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2740DB85-A635-43C8-AE45-C6013C030F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="102">
   <si>
     <t>Mã hóa đơn: 1</t>
   </si>
@@ -40,10 +40,10 @@
     <t>Mã KM: 1</t>
   </si>
   <si>
-    <t>Mã NV: 12</t>
-  </si>
-  <si>
-    <t>Mã KH: 21</t>
+    <t>Mã NV: 1</t>
+  </si>
+  <si>
+    <t>Mã KH: 11</t>
   </si>
   <si>
     <t>Mã Lô Hàng</t>
@@ -70,40 +70,262 @@
     <t>Mã KM: 2</t>
   </si>
   <si>
-    <t>Mã KH: 22</t>
-  </si>
-  <si>
     <t>Mã hóa đơn: 3</t>
   </si>
   <si>
-    <t>Ngày xuất: 2025-11-04</t>
-  </si>
-  <si>
-    <t>Tổng tiền: 40000.00</t>
-  </si>
-  <si>
-    <t>Trạng thái: 0</t>
-  </si>
-  <si>
-    <t>Mã NV: 11</t>
+    <t>Ngày xuất: 2025-05-01</t>
+  </si>
+  <si>
+    <t>Mã KM: 3</t>
+  </si>
+  <si>
+    <t>Mã NV: 2</t>
+  </si>
+  <si>
+    <t>Mã KH: 12</t>
   </si>
   <si>
     <t>Mã hóa đơn: 4</t>
   </si>
   <si>
+    <t>Ngày xuất: 2025-05-02</t>
+  </si>
+  <si>
+    <t>Tổng tiền: 180000.00</t>
+  </si>
+  <si>
+    <t>Mã KM: 4</t>
+  </si>
+  <si>
     <t>Mã hóa đơn: 5</t>
   </si>
   <si>
-    <t>Ngày xuất: 2025-11-05</t>
-  </si>
-  <si>
-    <t>Tổng tiền: 38000.00</t>
+    <t>Ngày xuất: 2025-05-03</t>
+  </si>
+  <si>
+    <t>Tổng tiền: 220000.00</t>
+  </si>
+  <si>
+    <t>Mã KM: 5</t>
+  </si>
+  <si>
+    <t>Mã NV: 3</t>
+  </si>
+  <si>
+    <t>Mã KH: 13</t>
   </si>
   <si>
     <t>Mã hóa đơn: 6</t>
   </si>
   <si>
-    <t>Ngày xuất: 2025-11-09</t>
+    <t>Ngày xuất: 2025-05-04</t>
+  </si>
+  <si>
+    <t>Tổng tiền: 150000.00</t>
+  </si>
+  <si>
+    <t>Mã KM: 6</t>
+  </si>
+  <si>
+    <t>Mã hóa đơn: 7</t>
+  </si>
+  <si>
+    <t>Ngày xuất: 2025-05-05</t>
+  </si>
+  <si>
+    <t>Tổng tiền: 320000.00</t>
+  </si>
+  <si>
+    <t>Mã KM: 7</t>
+  </si>
+  <si>
+    <t>Mã NV: 4</t>
+  </si>
+  <si>
+    <t>Mã KH: 14</t>
+  </si>
+  <si>
+    <t>Mã hóa đơn: 8</t>
+  </si>
+  <si>
+    <t>Ngày xuất: 2025-05-06</t>
+  </si>
+  <si>
+    <t>Tổng tiền: 400000.00</t>
+  </si>
+  <si>
+    <t>Mã KM: 8</t>
+  </si>
+  <si>
+    <t>Mã hóa đơn: 9</t>
+  </si>
+  <si>
+    <t>Ngày xuất: 2025-05-07</t>
+  </si>
+  <si>
+    <t>Tổng tiền: 280000.00</t>
+  </si>
+  <si>
+    <t>Mã KM: 9</t>
+  </si>
+  <si>
+    <t>Mã NV: 5</t>
+  </si>
+  <si>
+    <t>Mã KH: 15</t>
+  </si>
+  <si>
+    <t>Mã hóa đơn: 10</t>
+  </si>
+  <si>
+    <t>Ngày xuất: 2025-05-08</t>
+  </si>
+  <si>
+    <t>Mã KM: 10</t>
+  </si>
+  <si>
+    <t>Mã hóa đơn: 11</t>
+  </si>
+  <si>
+    <t>Ngày xuất: 2025-05-09</t>
+  </si>
+  <si>
+    <t>Tổng tiền: 250000.00</t>
+  </si>
+  <si>
+    <t>Mã KM: 11</t>
+  </si>
+  <si>
+    <t>Mã NV: 6</t>
+  </si>
+  <si>
+    <t>Mã KH: 16</t>
+  </si>
+  <si>
+    <t>Mã hóa đơn: 12</t>
+  </si>
+  <si>
+    <t>Ngày xuất: 2025-05-10</t>
+  </si>
+  <si>
+    <t>Tổng tiền: 370000.00</t>
+  </si>
+  <si>
+    <t>Mã KM: 12</t>
+  </si>
+  <si>
+    <t>Mã hóa đơn: 13</t>
+  </si>
+  <si>
+    <t>Ngày xuất: 2025-05-11</t>
+  </si>
+  <si>
+    <t>Tổng tiền: 420000.00</t>
+  </si>
+  <si>
+    <t>Mã KM: 13</t>
+  </si>
+  <si>
+    <t>Mã NV: 7</t>
+  </si>
+  <si>
+    <t>Mã KH: 17</t>
+  </si>
+  <si>
+    <t>Mã hóa đơn: 14</t>
+  </si>
+  <si>
+    <t>Ngày xuất: 2025-05-12</t>
+  </si>
+  <si>
+    <t>Tổng tiền: 270000.00</t>
+  </si>
+  <si>
+    <t>Mã KM: 14</t>
+  </si>
+  <si>
+    <t>Mã hóa đơn: 15</t>
+  </si>
+  <si>
+    <t>Ngày xuất: 2025-05-13</t>
+  </si>
+  <si>
+    <t>Mã KM: 15</t>
+  </si>
+  <si>
+    <t>Mã NV: 8</t>
+  </si>
+  <si>
+    <t>Mã KH: 18</t>
+  </si>
+  <si>
+    <t>Mã hóa đơn: 16</t>
+  </si>
+  <si>
+    <t>Ngày xuất: 2025-05-14</t>
+  </si>
+  <si>
+    <t>Tổng tiền: 350000.00</t>
+  </si>
+  <si>
+    <t>Mã KM: 16</t>
+  </si>
+  <si>
+    <t>Mã hóa đơn: 17</t>
+  </si>
+  <si>
+    <t>Ngày xuất: 2025-05-15</t>
+  </si>
+  <si>
+    <t>Tổng tiền: 240000.00</t>
+  </si>
+  <si>
+    <t>Mã KM: 17</t>
+  </si>
+  <si>
+    <t>Mã NV: 9</t>
+  </si>
+  <si>
+    <t>Mã KH: 19</t>
+  </si>
+  <si>
+    <t>Mã hóa đơn: 18</t>
+  </si>
+  <si>
+    <t>Ngày xuất: 2025-05-16</t>
+  </si>
+  <si>
+    <t>Tổng tiền: 190000.00</t>
+  </si>
+  <si>
+    <t>Mã KM: 18</t>
+  </si>
+  <si>
+    <t>Mã hóa đơn: 19</t>
+  </si>
+  <si>
+    <t>Ngày xuất: 2025-05-17</t>
+  </si>
+  <si>
+    <t>Mã KM: 19</t>
+  </si>
+  <si>
+    <t>Mã NV: 10</t>
+  </si>
+  <si>
+    <t>Mã KH: 20</t>
+  </si>
+  <si>
+    <t>Mã hóa đơn: 20</t>
+  </si>
+  <si>
+    <t>Ngày xuất: 2025-05-18</t>
+  </si>
+  <si>
+    <t>Tổng tiền: 500000.00</t>
+  </si>
+  <si>
+    <t>Mã KM: 20</t>
   </si>
 </sst>
 </file>
@@ -481,20 +703,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -576,7 +798,7 @@
         <v>6</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -595,7 +817,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B7">
         <v>61</v>
@@ -609,28 +831,28 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="s">
+      <c r="G9" t="s">
         <v>19</v>
       </c>
-      <c r="D9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="H9" t="s">
         <v>20</v>
-      </c>
-      <c r="F9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -649,42 +871,42 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B11">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C11">
-        <v>25000</v>
+        <v>20000</v>
       </c>
       <c r="D11">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
       <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" t="s">
         <v>19</v>
       </c>
-      <c r="D13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="H13" t="s">
         <v>20</v>
-      </c>
-      <c r="F13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -703,166 +925,880 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
+        <v>56</v>
+      </c>
+      <c r="B15">
+        <v>64</v>
+      </c>
+      <c r="C15">
+        <v>15000</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>57</v>
+      </c>
+      <c r="B19">
+        <v>65</v>
+      </c>
+      <c r="C19">
+        <v>35000</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" t="s">
+        <v>29</v>
+      </c>
+      <c r="H21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>58</v>
+      </c>
+      <c r="B23">
+        <v>66</v>
+      </c>
+      <c r="C23">
+        <v>90000</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" t="s">
+        <v>38</v>
+      </c>
+      <c r="G25" t="s">
+        <v>39</v>
+      </c>
+      <c r="H25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>59</v>
+      </c>
+      <c r="B27">
+        <v>67</v>
+      </c>
+      <c r="C27">
+        <v>80000</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" t="s">
+        <v>44</v>
+      </c>
+      <c r="G29" t="s">
+        <v>39</v>
+      </c>
+      <c r="H29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>60</v>
+      </c>
+      <c r="B31">
+        <v>68</v>
+      </c>
+      <c r="C31">
+        <v>95000</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" t="s">
+        <v>48</v>
+      </c>
+      <c r="G33" t="s">
+        <v>49</v>
+      </c>
+      <c r="H33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>61</v>
+      </c>
+      <c r="B35">
+        <v>69</v>
+      </c>
+      <c r="C35">
+        <v>50000</v>
+      </c>
+      <c r="D35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>51</v>
       </c>
-      <c r="B15">
+      <c r="B37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" t="s">
+        <v>33</v>
+      </c>
+      <c r="D37" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" t="s">
+        <v>53</v>
+      </c>
+      <c r="G37" t="s">
+        <v>49</v>
+      </c>
+      <c r="H37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>62</v>
+      </c>
+      <c r="B39">
+        <v>70</v>
+      </c>
+      <c r="C39">
+        <v>25000</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" t="s">
+        <v>57</v>
+      </c>
+      <c r="G41" t="s">
+        <v>58</v>
+      </c>
+      <c r="H41" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>63</v>
+      </c>
+      <c r="B43">
+        <v>71</v>
+      </c>
+      <c r="C43">
+        <v>70000</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" t="s">
         <v>61</v>
       </c>
-      <c r="C15">
-        <v>25000</v>
-      </c>
-      <c r="D15">
+      <c r="C45" t="s">
+        <v>62</v>
+      </c>
+      <c r="D45" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45" t="s">
+        <v>4</v>
+      </c>
+      <c r="F45" t="s">
+        <v>63</v>
+      </c>
+      <c r="G45" t="s">
+        <v>58</v>
+      </c>
+      <c r="H45" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>64</v>
+      </c>
+      <c r="B47">
+        <v>72</v>
+      </c>
+      <c r="C47">
+        <v>120000</v>
+      </c>
+      <c r="D47">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>52</v>
-      </c>
-      <c r="B16">
-        <v>62</v>
-      </c>
-      <c r="C16">
-        <v>15000</v>
-      </c>
-      <c r="D16">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>64</v>
+      </c>
+      <c r="B49" t="s">
+        <v>65</v>
+      </c>
+      <c r="C49" t="s">
+        <v>66</v>
+      </c>
+      <c r="D49" t="s">
+        <v>14</v>
+      </c>
+      <c r="E49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F49" t="s">
+        <v>67</v>
+      </c>
+      <c r="G49" t="s">
+        <v>68</v>
+      </c>
+      <c r="H49" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>65</v>
+      </c>
+      <c r="B51">
+        <v>73</v>
+      </c>
+      <c r="C51">
+        <v>30000</v>
+      </c>
+      <c r="D51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>70</v>
+      </c>
+      <c r="B53" t="s">
+        <v>71</v>
+      </c>
+      <c r="C53" t="s">
+        <v>72</v>
+      </c>
+      <c r="D53" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F53" t="s">
+        <v>73</v>
+      </c>
+      <c r="G53" t="s">
+        <v>68</v>
+      </c>
+      <c r="H53" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>66</v>
+      </c>
+      <c r="B55">
+        <v>74</v>
+      </c>
+      <c r="C55">
+        <v>45000</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>74</v>
+      </c>
+      <c r="B57" t="s">
+        <v>75</v>
+      </c>
+      <c r="C57" t="s">
+        <v>23</v>
+      </c>
+      <c r="D57" t="s">
+        <v>14</v>
+      </c>
+      <c r="E57" t="s">
+        <v>4</v>
+      </c>
+      <c r="F57" t="s">
+        <v>76</v>
+      </c>
+      <c r="G57" t="s">
+        <v>77</v>
+      </c>
+      <c r="H57" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>67</v>
+      </c>
+      <c r="B59">
+        <v>75</v>
+      </c>
+      <c r="C59">
+        <v>40000</v>
+      </c>
+      <c r="D59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>79</v>
+      </c>
+      <c r="B61" t="s">
+        <v>80</v>
+      </c>
+      <c r="C61" t="s">
+        <v>81</v>
+      </c>
+      <c r="D61" t="s">
+        <v>3</v>
+      </c>
+      <c r="E61" t="s">
+        <v>4</v>
+      </c>
+      <c r="F61" t="s">
+        <v>82</v>
+      </c>
+      <c r="G61" t="s">
+        <v>77</v>
+      </c>
+      <c r="H61" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>68</v>
+      </c>
+      <c r="B63">
+        <v>76</v>
+      </c>
+      <c r="C63">
+        <v>85000</v>
+      </c>
+      <c r="D63">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" t="s">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>83</v>
+      </c>
+      <c r="B65" t="s">
+        <v>84</v>
+      </c>
+      <c r="C65" t="s">
+        <v>85</v>
+      </c>
+      <c r="D65" t="s">
         <v>14</v>
       </c>
-      <c r="E18" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" t="s">
-        <v>5</v>
-      </c>
-      <c r="G18" t="s">
-        <v>21</v>
-      </c>
-      <c r="H18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>51</v>
-      </c>
-      <c r="B20">
-        <v>61</v>
-      </c>
-      <c r="C20">
-        <v>25000</v>
-      </c>
-      <c r="D20">
+      <c r="E65" t="s">
+        <v>4</v>
+      </c>
+      <c r="F65" t="s">
+        <v>86</v>
+      </c>
+      <c r="G65" t="s">
+        <v>87</v>
+      </c>
+      <c r="H65" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>69</v>
+      </c>
+      <c r="B67">
+        <v>77</v>
+      </c>
+      <c r="C67">
+        <v>90000</v>
+      </c>
+      <c r="D67">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>52</v>
-      </c>
-      <c r="B21">
-        <v>62</v>
-      </c>
-      <c r="C21">
-        <v>15000</v>
-      </c>
-      <c r="D21">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>89</v>
+      </c>
+      <c r="B69" t="s">
+        <v>90</v>
+      </c>
+      <c r="C69" t="s">
+        <v>91</v>
+      </c>
+      <c r="D69" t="s">
+        <v>3</v>
+      </c>
+      <c r="E69" t="s">
+        <v>4</v>
+      </c>
+      <c r="F69" t="s">
+        <v>92</v>
+      </c>
+      <c r="G69" t="s">
+        <v>87</v>
+      </c>
+      <c r="H69" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>78</v>
+      </c>
+      <c r="C71">
+        <v>350000</v>
+      </c>
+      <c r="D71">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" t="s">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>93</v>
+      </c>
+      <c r="B73" t="s">
+        <v>94</v>
+      </c>
+      <c r="C73" t="s">
+        <v>47</v>
+      </c>
+      <c r="D73" t="s">
         <v>14</v>
       </c>
-      <c r="E23" t="s">
-        <v>4</v>
-      </c>
-      <c r="F23" t="s">
-        <v>5</v>
-      </c>
-      <c r="G23" t="s">
-        <v>6</v>
-      </c>
-      <c r="H23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>51</v>
-      </c>
-      <c r="B25">
-        <v>61</v>
-      </c>
-      <c r="C25">
-        <v>25000</v>
-      </c>
-      <c r="D25">
+      <c r="E73" t="s">
+        <v>4</v>
+      </c>
+      <c r="F73" t="s">
+        <v>95</v>
+      </c>
+      <c r="G73" t="s">
+        <v>96</v>
+      </c>
+      <c r="H73" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>71</v>
+      </c>
+      <c r="B75">
+        <v>79</v>
+      </c>
+      <c r="C75">
+        <v>220000</v>
+      </c>
+      <c r="D75">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>52</v>
-      </c>
-      <c r="B26">
-        <v>62</v>
-      </c>
-      <c r="C26">
-        <v>15000</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>98</v>
+      </c>
+      <c r="B77" t="s">
+        <v>99</v>
+      </c>
+      <c r="C77" t="s">
+        <v>100</v>
+      </c>
+      <c r="D77" t="s">
+        <v>3</v>
+      </c>
+      <c r="E77" t="s">
+        <v>4</v>
+      </c>
+      <c r="F77" t="s">
+        <v>101</v>
+      </c>
+      <c r="G77" t="s">
+        <v>96</v>
+      </c>
+      <c r="H77" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>72</v>
+      </c>
+      <c r="B79">
+        <v>80</v>
+      </c>
+      <c r="C79">
+        <v>40000</v>
+      </c>
+      <c r="D79">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>